<commit_message>
wip powerpoint + timescheet
</commit_message>
<xml_diff>
--- a/docs/timesheet_Basiel_Smitz.xlsx
+++ b/docs/timesheet_Basiel_Smitz.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
   <si>
     <t>Datum</t>
   </si>
@@ -76,6 +76,33 @@
   </si>
   <si>
     <t>Database design</t>
+  </si>
+  <si>
+    <t>Powerpoint</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>opzetten laravel omgeving</t>
+  </si>
+  <si>
+    <t>Style tiles</t>
+  </si>
+  <si>
+    <t>Bespreking style tiles, wireframes, ...</t>
+  </si>
+  <si>
+    <t>Database migrations</t>
+  </si>
+  <si>
+    <t>Visual designs</t>
+  </si>
+  <si>
+    <t>Dossier in MD</t>
+  </si>
+  <si>
+    <t>2.5</t>
   </si>
 </sst>
 </file>
@@ -482,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,6 +686,125 @@
       </c>
       <c r="F9" s="2"/>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>42797</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>42802</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>42804</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>42807</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>42808</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>42810</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>42810</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E9"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>